<commit_message>
Backed out changeset: feed2fa274b1 Backward compatibility issue. It will be reimplemented in the next release.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test/rules/functionality/Arithmetic.xlsx
+++ b/DEV/org.openl.test/test/rules/functionality/Arithmetic.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="71">
   <si>
     <t>Result</t>
   </si>
@@ -202,7 +202,31 @@
     <t>multiply:IntValue</t>
   </si>
   <si>
-    <t>divide:DoubleValue</t>
+    <t>divide:byte</t>
+  </si>
+  <si>
+    <t>divide:short</t>
+  </si>
+  <si>
+    <t>divide:int</t>
+  </si>
+  <si>
+    <t>divide:long</t>
+  </si>
+  <si>
+    <t>divide:float</t>
+  </si>
+  <si>
+    <t>divide:BigInteger</t>
+  </si>
+  <si>
+    <t>divide:IntValue</t>
+  </si>
+  <si>
+    <t>_res_.$v$divide</t>
+  </si>
+  <si>
+    <t>_res_.$v$divide (7)</t>
   </si>
 </sst>
 </file>
@@ -665,7 +689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -675,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="O86" sqref="O86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -763,7 +787,7 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
@@ -779,10 +803,10 @@
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="H10" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="J10" s="4">
-        <v>0.66666666666666596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
@@ -888,7 +912,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3</v>
@@ -913,11 +937,11 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="4">
-        <v>0.66666666666666596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
@@ -1027,7 +1051,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>3</v>
@@ -1052,11 +1076,11 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="4">
-        <v>0.66666666666666596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
@@ -1166,7 +1190,7 @@
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>3</v>
@@ -1191,11 +1215,11 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="4">
-        <v>0.66666666666666596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
@@ -1305,7 +1329,7 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>3</v>
@@ -1330,11 +1354,11 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="4">
-        <v>0.66666666666666596</v>
+        <v>0.6666666</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
@@ -1567,7 +1591,7 @@
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>3</v>
@@ -1584,7 +1608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="2:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
       <c r="C64" s="2"/>
       <c r="D64" s="1"/>
@@ -1592,11 +1616,11 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="I64" s="1"/>
-      <c r="J64" s="4" t="s">
-        <v>55</v>
+      <c r="J64" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.2">
@@ -1829,7 +1853,7 @@
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>3</v>
@@ -1854,11 +1878,11 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="I84" s="1"/>
       <c r="J84" s="4">
-        <v>0.66666666666666596</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>